<commit_message>
added: value validation starter import and massive add massive add functionality test data sheet with errors starter to array function (creates an array out of the starter entity)
finished:
starter import

changed:
some UI and texts
</commit_message>
<xml_diff>
--- a/web/test_data.xlsx
+++ b/web/test_data.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="705" uniqueCount="220">
   <si>
     <t>Baroncelli</t>
   </si>
@@ -681,12 +681,6 @@
   </si>
   <si>
     <t>K1</t>
-  </si>
-  <si>
-    <t>Mathias</t>
-  </si>
-  <si>
-    <t>Scherer</t>
   </si>
 </sst>
 </file>
@@ -757,7 +751,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -926,31 +920,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="medium">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1116,17 +1090,6 @@
       <alignment horizontal="right" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -1431,10 +1394,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F297"/>
+  <dimension ref="A1:F141"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A289" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J293" sqref="J293"/>
+    <sheetView tabSelected="1" topLeftCell="A203" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C220" sqref="C220"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4261,3048 +4224,6 @@
         <v>215</v>
       </c>
       <c r="F141" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="143" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A143" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="B143" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="C143" s="46">
-        <v>1996</v>
-      </c>
-      <c r="D143" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E143" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F143" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A144" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B144" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="C144" s="37">
-        <v>1996</v>
-      </c>
-      <c r="D144" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E144" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F144" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A145" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="B145" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="C145" s="41">
-        <v>1998</v>
-      </c>
-      <c r="D145" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E145" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F145" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A146" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="B146" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="C146" s="61">
-        <v>1996</v>
-      </c>
-      <c r="D146" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E146" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F146" s="60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A147" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B147" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="C147" s="61">
-        <v>1996</v>
-      </c>
-      <c r="D147" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E147" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F147" s="62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A148" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="B148" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="C148" s="61">
-        <v>1997</v>
-      </c>
-      <c r="D148" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E148" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F148" s="62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A149" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="B149" s="54" t="s">
-        <v>138</v>
-      </c>
-      <c r="C149" s="57">
-        <v>1998</v>
-      </c>
-      <c r="D149" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E149" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F149" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A150" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="B150" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C150" s="57">
-        <v>1998</v>
-      </c>
-      <c r="D150" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E150" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F150" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A151" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="B151" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C151" s="57">
-        <v>1999</v>
-      </c>
-      <c r="D151" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E151" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F151" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A152" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="B152" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C152" s="58">
-        <v>1999</v>
-      </c>
-      <c r="D152" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E152" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F152" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="156" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A156" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="B156" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C156" s="3">
-        <v>2004</v>
-      </c>
-      <c r="D156" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E156" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F156" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A157" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B157" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C157" s="3">
-        <v>2003</v>
-      </c>
-      <c r="D157" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E157" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F157" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A158" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B158" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="C158" s="5">
-        <v>2002</v>
-      </c>
-      <c r="D158" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E158" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F158" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A159" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="B159" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C159" s="7">
-        <v>2001</v>
-      </c>
-      <c r="D159" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E159" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F159" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A160" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B160" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C160" s="9">
-        <v>2002</v>
-      </c>
-      <c r="D160" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E160" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F160" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A161" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="B161" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C161" s="9">
-        <v>2001</v>
-      </c>
-      <c r="D161" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E161" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F161" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A162" s="25" t="s">
-        <v>89</v>
-      </c>
-      <c r="B162" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="C162" s="27">
-        <v>2003</v>
-      </c>
-      <c r="D162" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E162" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F162" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A163" s="28" t="s">
-        <v>92</v>
-      </c>
-      <c r="B163" s="28" t="s">
-        <v>91</v>
-      </c>
-      <c r="C163" s="29">
-        <v>2003</v>
-      </c>
-      <c r="D163" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E163" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F163" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A164" s="28" t="s">
-        <v>93</v>
-      </c>
-      <c r="B164" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="C164" s="29">
-        <v>2003</v>
-      </c>
-      <c r="D164" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E164" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F164" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A165" s="28" t="s">
-        <v>95</v>
-      </c>
-      <c r="B165" s="28" t="s">
-        <v>94</v>
-      </c>
-      <c r="C165" s="29">
-        <v>2004</v>
-      </c>
-      <c r="D165" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E165" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F165" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A166" s="28" t="s">
-        <v>97</v>
-      </c>
-      <c r="B166" s="28" t="s">
-        <v>96</v>
-      </c>
-      <c r="C166" s="29">
-        <v>2004</v>
-      </c>
-      <c r="D166" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E166" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F166" s="26" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A167" s="31" t="s">
-        <v>89</v>
-      </c>
-      <c r="B167" s="31" t="s">
-        <v>98</v>
-      </c>
-      <c r="C167" s="34">
-        <v>2004</v>
-      </c>
-      <c r="D167" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E167" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F167" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A168" s="31" t="s">
-        <v>100</v>
-      </c>
-      <c r="B168" s="31" t="s">
-        <v>99</v>
-      </c>
-      <c r="C168" s="34">
-        <v>2004</v>
-      </c>
-      <c r="D168" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E168" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F168" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="169" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A169" s="31" t="s">
-        <v>102</v>
-      </c>
-      <c r="B169" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="C169" s="34">
-        <v>2005</v>
-      </c>
-      <c r="D169" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E169" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F169" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="170" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A170" s="35" t="s">
-        <v>141</v>
-      </c>
-      <c r="B170" s="35" t="s">
-        <v>142</v>
-      </c>
-      <c r="C170" s="36">
-        <v>2005</v>
-      </c>
-      <c r="D170" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E170" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F170" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="171" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A171" s="31" t="s">
-        <v>144</v>
-      </c>
-      <c r="B171" s="31" t="s">
-        <v>62</v>
-      </c>
-      <c r="C171" s="36">
-        <v>2004</v>
-      </c>
-      <c r="D171" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E171" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F171" s="32" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="172" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A172" s="38" t="s">
-        <v>146</v>
-      </c>
-      <c r="B172" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C172" s="40">
-        <v>2005</v>
-      </c>
-      <c r="D172" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E172" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F172" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="173" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A173" s="38" t="s">
-        <v>110</v>
-      </c>
-      <c r="B173" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C173" s="41">
-        <v>2003</v>
-      </c>
-      <c r="D173" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E173" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F173" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="174" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A174" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="B174" s="38" t="s">
-        <v>147</v>
-      </c>
-      <c r="C174" s="41">
-        <v>2003</v>
-      </c>
-      <c r="D174" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E174" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F174" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="175" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A175" s="38" t="s">
-        <v>149</v>
-      </c>
-      <c r="B175" s="38" t="s">
-        <v>148</v>
-      </c>
-      <c r="C175" s="41">
-        <v>2006</v>
-      </c>
-      <c r="D175" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E175" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F175" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="176" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A176" s="38" t="s">
-        <v>151</v>
-      </c>
-      <c r="B176" s="38" t="s">
-        <v>150</v>
-      </c>
-      <c r="C176" s="41">
-        <v>2004</v>
-      </c>
-      <c r="D176" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E176" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F176" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="177" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A177" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="B177" s="18" t="s">
-        <v>171</v>
-      </c>
-      <c r="C177" s="20">
-        <v>2000</v>
-      </c>
-      <c r="D177" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E177" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F177" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A178" s="21" t="s">
-        <v>175</v>
-      </c>
-      <c r="B178" s="21" t="s">
-        <v>174</v>
-      </c>
-      <c r="C178" s="20">
-        <v>2000</v>
-      </c>
-      <c r="D178" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E178" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F178" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="179" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A179" s="21" t="s">
-        <v>146</v>
-      </c>
-      <c r="B179" s="21" t="s">
-        <v>176</v>
-      </c>
-      <c r="C179" s="20">
-        <v>2001</v>
-      </c>
-      <c r="D179" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E179" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F179" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A180" s="21" t="s">
-        <v>178</v>
-      </c>
-      <c r="B180" s="21" t="s">
-        <v>177</v>
-      </c>
-      <c r="C180" s="20">
-        <v>2003</v>
-      </c>
-      <c r="D180" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E180" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F180" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="181" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A181" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="B181" s="21" t="s">
-        <v>179</v>
-      </c>
-      <c r="C181" s="20">
-        <v>2003</v>
-      </c>
-      <c r="D181" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E181" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F181" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A182" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="B182" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C182" s="24">
-        <v>2003</v>
-      </c>
-      <c r="D182" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E182" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="F182" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A183" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B183" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="C183" s="14">
-        <v>2003</v>
-      </c>
-      <c r="D183" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E183" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F183" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A184" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B184" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C184" s="14">
-        <v>2004</v>
-      </c>
-      <c r="D184" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E184" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F184" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="185" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A185" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B185" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="C185" s="12">
-        <v>2000</v>
-      </c>
-      <c r="D185" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E185" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F185" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="186" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A186" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B186" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C186" s="14">
-        <v>2000</v>
-      </c>
-      <c r="D186" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E186" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F186" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="187" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A187" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="B187" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C187" s="14">
-        <v>1999</v>
-      </c>
-      <c r="D187" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E187" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F187" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="188" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A188" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B188" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="C188" s="14">
-        <v>2000</v>
-      </c>
-      <c r="D188" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E188" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F188" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A189" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="B189" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="C189" s="14">
-        <v>2000</v>
-      </c>
-      <c r="D189" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E189" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F189" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A190" s="13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B190" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="C190" s="14">
-        <v>1999</v>
-      </c>
-      <c r="D190" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E190" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F190" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A191" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B191" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="C191" s="43">
-        <v>2000</v>
-      </c>
-      <c r="D191" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E191" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F191" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A192" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B192" s="42" t="s">
-        <v>48</v>
-      </c>
-      <c r="C192" s="43">
-        <v>2001</v>
-      </c>
-      <c r="D192" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E192" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F192" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="193" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A193" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="B193" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="C193" s="43">
-        <v>1998</v>
-      </c>
-      <c r="D193" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E193" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F193" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="194" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A194" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="B194" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="C194" s="43">
-        <v>1998</v>
-      </c>
-      <c r="D194" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E194" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F194" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="195" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A195" s="42" t="s">
-        <v>54</v>
-      </c>
-      <c r="B195" s="42" t="s">
-        <v>53</v>
-      </c>
-      <c r="C195" s="43">
-        <v>1999</v>
-      </c>
-      <c r="D195" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E195" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F195" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="196" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A196" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B196" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="C196" s="43">
-        <v>1999</v>
-      </c>
-      <c r="D196" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E196" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F196" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="197" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A197" s="25" t="s">
-        <v>73</v>
-      </c>
-      <c r="B197" s="25" t="s">
-        <v>72</v>
-      </c>
-      <c r="C197" s="27">
-        <v>2003</v>
-      </c>
-      <c r="D197" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E197" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F197" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="198" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="B198" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="C198" s="34">
-        <v>2001</v>
-      </c>
-      <c r="D198" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E198" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F198" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="199" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A199" s="31" t="s">
-        <v>104</v>
-      </c>
-      <c r="B199" s="31" t="s">
-        <v>103</v>
-      </c>
-      <c r="C199" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D199" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E199" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F199" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="200" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A200" s="31" t="s">
-        <v>106</v>
-      </c>
-      <c r="B200" s="31" t="s">
-        <v>105</v>
-      </c>
-      <c r="C200" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D200" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E200" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F200" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="201" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A201" s="31" t="s">
-        <v>108</v>
-      </c>
-      <c r="B201" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="C201" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D201" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E201" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F201" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="202" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A202" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="B202" s="31" t="s">
-        <v>109</v>
-      </c>
-      <c r="C202" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D202" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E202" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F202" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="203" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A203" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="B203" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="C203" s="34">
-        <v>2003</v>
-      </c>
-      <c r="D203" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E203" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F203" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="204" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A204" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="B204" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C204" s="34">
-        <v>2003</v>
-      </c>
-      <c r="D204" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E204" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F204" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="205" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="31" t="s">
-        <v>115</v>
-      </c>
-      <c r="B205" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="C205" s="34">
-        <v>2003</v>
-      </c>
-      <c r="D205" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E205" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F205" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="206" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="31" t="s">
-        <v>116</v>
-      </c>
-      <c r="B206" s="31" t="s">
-        <v>27</v>
-      </c>
-      <c r="C206" s="34">
-        <v>2003</v>
-      </c>
-      <c r="D206" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E206" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F206" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="207" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A207" s="45" t="s">
-        <v>58</v>
-      </c>
-      <c r="B207" s="44" t="s">
-        <v>212</v>
-      </c>
-      <c r="C207" s="46">
-        <v>2000</v>
-      </c>
-      <c r="D207" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E207" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F207" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="208" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="38" t="s">
-        <v>152</v>
-      </c>
-      <c r="B208" s="38" t="s">
-        <v>145</v>
-      </c>
-      <c r="C208" s="41">
-        <v>2002</v>
-      </c>
-      <c r="D208" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E208" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F208" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="209" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A209" s="38" t="s">
-        <v>1</v>
-      </c>
-      <c r="B209" s="38" t="s">
-        <v>153</v>
-      </c>
-      <c r="C209" s="41">
-        <v>2002</v>
-      </c>
-      <c r="D209" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E209" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F209" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="210" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A210" s="38" t="s">
-        <v>155</v>
-      </c>
-      <c r="B210" s="38" t="s">
-        <v>154</v>
-      </c>
-      <c r="C210" s="41">
-        <v>2003</v>
-      </c>
-      <c r="D210" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E210" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F210" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="211" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A211" s="38" t="s">
-        <v>157</v>
-      </c>
-      <c r="B211" s="38" t="s">
-        <v>156</v>
-      </c>
-      <c r="C211" s="41">
-        <v>2003</v>
-      </c>
-      <c r="D211" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E211" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F211" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="212" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A212" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="B212" s="38" t="s">
-        <v>180</v>
-      </c>
-      <c r="C212" s="41">
-        <v>2001</v>
-      </c>
-      <c r="D212" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E212" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F212" s="39" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="213" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A213" s="38" t="s">
-        <v>182</v>
-      </c>
-      <c r="B213" s="38" t="s">
-        <v>181</v>
-      </c>
-      <c r="C213" s="41">
-        <v>2002</v>
-      </c>
-      <c r="D213" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E213" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F213" s="39" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="214" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="38" t="s">
-        <v>184</v>
-      </c>
-      <c r="B214" s="38" t="s">
-        <v>183</v>
-      </c>
-      <c r="C214" s="41">
-        <v>2000</v>
-      </c>
-      <c r="D214" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E214" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F214" s="39" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="215" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A215" s="22" t="s">
-        <v>170</v>
-      </c>
-      <c r="B215" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C215" s="24">
-        <v>2001</v>
-      </c>
-      <c r="D215" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E215" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F215" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="216" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A216" s="22" t="s">
-        <v>196</v>
-      </c>
-      <c r="B216" s="22" t="s">
-        <v>195</v>
-      </c>
-      <c r="C216" s="24">
-        <v>2002</v>
-      </c>
-      <c r="D216" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E216" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F216" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="217" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A217" s="22" t="s">
-        <v>198</v>
-      </c>
-      <c r="B217" s="22" t="s">
-        <v>197</v>
-      </c>
-      <c r="C217" s="24">
-        <v>2003</v>
-      </c>
-      <c r="D217" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E217" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F217" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="218" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A218" s="22" t="s">
-        <v>38</v>
-      </c>
-      <c r="B218" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C218" s="24">
-        <v>2001</v>
-      </c>
-      <c r="D218" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E218" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F218" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="219" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A219" s="22" t="s">
-        <v>83</v>
-      </c>
-      <c r="B219" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C219" s="24">
-        <v>2000</v>
-      </c>
-      <c r="D219" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E219" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F219" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="220" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A220" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="B220" s="22" t="s">
-        <v>147</v>
-      </c>
-      <c r="C220" s="24">
-        <v>2001</v>
-      </c>
-      <c r="D220" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E220" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F220" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="221" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A221" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="B221" s="22" t="s">
-        <v>200</v>
-      </c>
-      <c r="C221" s="24">
-        <v>2000</v>
-      </c>
-      <c r="D221" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E221" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F221" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="222" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A222" s="22" t="s">
-        <v>201</v>
-      </c>
-      <c r="B222" s="22" t="s">
-        <v>46</v>
-      </c>
-      <c r="C222" s="24">
-        <v>2002</v>
-      </c>
-      <c r="D222" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E222" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F222" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="223" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A223" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="B223" s="22" t="s">
-        <v>202</v>
-      </c>
-      <c r="C223" s="24">
-        <v>2000</v>
-      </c>
-      <c r="D223" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E223" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="F223" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="224" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A224" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B224" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="C224" s="14">
-        <v>2002</v>
-      </c>
-      <c r="D224" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E224" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F224" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="225" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A225" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B225" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="C225" s="14">
-        <v>2002</v>
-      </c>
-      <c r="D225" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E225" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F225" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="226" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A226" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="B226" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="C226" s="14">
-        <v>2000</v>
-      </c>
-      <c r="D226" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E226" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F226" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="227" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A227" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B227" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C227" s="14">
-        <v>2001</v>
-      </c>
-      <c r="D227" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E227" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F227" s="11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="228" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A228" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="B228" s="16" t="s">
-        <v>57</v>
-      </c>
-      <c r="C228" s="17">
-        <v>1998</v>
-      </c>
-      <c r="D228" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E228" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F228" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="229" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A229" s="16" t="s">
-        <v>38</v>
-      </c>
-      <c r="B229" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="C229" s="17">
-        <v>1999</v>
-      </c>
-      <c r="D229" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E229" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F229" s="11" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="230" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A230" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="B230" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="C230" s="27">
-        <v>2000</v>
-      </c>
-      <c r="D230" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E230" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F230" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="231" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A231" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B231" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="C231" s="29">
-        <v>2002</v>
-      </c>
-      <c r="D231" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E231" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F231" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="232" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A232" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B232" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C232" s="29">
-        <v>1993</v>
-      </c>
-      <c r="D232" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E232" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F232" s="26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="233" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A233" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="B233" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C233" s="29">
-        <v>2003</v>
-      </c>
-      <c r="D233" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E233" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F233" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="28" t="s">
-        <v>77</v>
-      </c>
-      <c r="B234" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="C234" s="29">
-        <v>2001</v>
-      </c>
-      <c r="D234" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E234" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F234" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="235" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A235" s="28" t="s">
-        <v>78</v>
-      </c>
-      <c r="B235" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C235" s="29">
-        <v>2001</v>
-      </c>
-      <c r="D235" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E235" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F235" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="236" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A236" s="31" t="s">
-        <v>118</v>
-      </c>
-      <c r="B236" s="31" t="s">
-        <v>117</v>
-      </c>
-      <c r="C236" s="34">
-        <v>2000</v>
-      </c>
-      <c r="D236" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E236" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F236" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="237" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A237" s="31" t="s">
-        <v>119</v>
-      </c>
-      <c r="B237" s="31" t="s">
-        <v>91</v>
-      </c>
-      <c r="C237" s="34">
-        <v>2001</v>
-      </c>
-      <c r="D237" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E237" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F237" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="238" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A238" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="B238" s="31" t="s">
-        <v>120</v>
-      </c>
-      <c r="C238" s="34">
-        <v>2001</v>
-      </c>
-      <c r="D238" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E238" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F238" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="239" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A239" s="31" t="s">
-        <v>123</v>
-      </c>
-      <c r="B239" s="31" t="s">
-        <v>122</v>
-      </c>
-      <c r="C239" s="34">
-        <v>2001</v>
-      </c>
-      <c r="D239" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E239" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F239" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="240" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A240" s="31" t="s">
-        <v>125</v>
-      </c>
-      <c r="B240" s="31" t="s">
-        <v>124</v>
-      </c>
-      <c r="C240" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D240" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E240" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F240" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="241" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A241" s="31" t="s">
-        <v>4</v>
-      </c>
-      <c r="B241" s="31" t="s">
-        <v>126</v>
-      </c>
-      <c r="C241" s="34">
-        <v>2002</v>
-      </c>
-      <c r="D241" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E241" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F241" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="242" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A242" s="38" t="s">
-        <v>135</v>
-      </c>
-      <c r="B242" s="38" t="s">
-        <v>158</v>
-      </c>
-      <c r="C242" s="41">
-        <v>2000</v>
-      </c>
-      <c r="D242" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E242" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F242" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="243" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A243" s="38" t="s">
-        <v>160</v>
-      </c>
-      <c r="B243" s="38" t="s">
-        <v>159</v>
-      </c>
-      <c r="C243" s="41">
-        <v>2001</v>
-      </c>
-      <c r="D243" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E243" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F243" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="244" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A244" s="38" t="s">
-        <v>161</v>
-      </c>
-      <c r="B244" s="38" t="s">
-        <v>59</v>
-      </c>
-      <c r="C244" s="41">
-        <v>2000</v>
-      </c>
-      <c r="D244" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E244" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F244" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="245" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A245" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="B245" s="38" t="s">
-        <v>162</v>
-      </c>
-      <c r="C245" s="41">
-        <v>1999</v>
-      </c>
-      <c r="D245" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E245" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F245" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="246" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A246" s="38" t="s">
-        <v>164</v>
-      </c>
-      <c r="B246" s="38" t="s">
-        <v>163</v>
-      </c>
-      <c r="C246" s="41">
-        <v>2000</v>
-      </c>
-      <c r="D246" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E246" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F246" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="247" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A247" s="21" t="s">
-        <v>186</v>
-      </c>
-      <c r="B247" s="21" t="s">
-        <v>185</v>
-      </c>
-      <c r="C247" s="20">
-        <v>2001</v>
-      </c>
-      <c r="D247" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E247" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F247" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="248" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A248" s="21" t="s">
-        <v>95</v>
-      </c>
-      <c r="B248" s="21" t="s">
-        <v>187</v>
-      </c>
-      <c r="C248" s="20">
-        <v>2001</v>
-      </c>
-      <c r="D248" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E248" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F248" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="249" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A249" s="21" t="s">
-        <v>6</v>
-      </c>
-      <c r="B249" s="21" t="s">
-        <v>188</v>
-      </c>
-      <c r="C249" s="20">
-        <v>1998</v>
-      </c>
-      <c r="D249" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E249" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F249" s="19" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="250" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A250" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="B250" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="C250" s="24">
-        <v>2000</v>
-      </c>
-      <c r="D250" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E250" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F250" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="251" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A251" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="B251" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C251" s="24">
-        <v>1999</v>
-      </c>
-      <c r="D251" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E251" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F251" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="252" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A252" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="B252" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="C252" s="24">
-        <v>2000</v>
-      </c>
-      <c r="D252" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E252" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="F252" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="253" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A253" s="15" t="s">
-        <v>190</v>
-      </c>
-      <c r="B253" s="15" t="s">
-        <v>189</v>
-      </c>
-      <c r="C253" s="51">
-        <v>1998</v>
-      </c>
-      <c r="D253" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E253" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F253" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="254" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A254" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="B254" s="13" t="s">
-        <v>191</v>
-      </c>
-      <c r="C254" s="51">
-        <v>2000</v>
-      </c>
-      <c r="D254" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E254" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F254" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="255" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A255" s="13" t="s">
-        <v>182</v>
-      </c>
-      <c r="B255" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="C255" s="51">
-        <v>2000</v>
-      </c>
-      <c r="D255" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E255" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F255" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="256" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A256" s="13" t="s">
-        <v>45</v>
-      </c>
-      <c r="B256" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C256" s="51">
-        <v>1997</v>
-      </c>
-      <c r="D256" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E256" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F256" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="257" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A257" s="13" t="s">
-        <v>192</v>
-      </c>
-      <c r="B257" s="13" t="s">
-        <v>89</v>
-      </c>
-      <c r="C257" s="51">
-        <v>1998</v>
-      </c>
-      <c r="D257" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E257" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F257" s="11" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="258" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A258" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="B258" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="C258" s="29">
-        <v>1998</v>
-      </c>
-      <c r="D258" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E258" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F258" s="26" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="259" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A259" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="B259" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="C259" s="29">
-        <v>2000</v>
-      </c>
-      <c r="D259" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E259" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F259" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="260" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A260" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="B260" s="28" t="s">
-        <v>81</v>
-      </c>
-      <c r="C260" s="29">
-        <v>2000</v>
-      </c>
-      <c r="D260" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E260" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F260" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="261" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A261" s="28" t="s">
-        <v>83</v>
-      </c>
-      <c r="B261" s="28" t="s">
-        <v>82</v>
-      </c>
-      <c r="C261" s="29">
-        <v>1998</v>
-      </c>
-      <c r="D261" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E261" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F261" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="262" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A262" s="28" t="s">
-        <v>85</v>
-      </c>
-      <c r="B262" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="C262" s="29">
-        <v>1997</v>
-      </c>
-      <c r="D262" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E262" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F262" s="26" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="263" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A263" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="B263" s="31" t="s">
-        <v>127</v>
-      </c>
-      <c r="C263" s="34">
-        <v>1998</v>
-      </c>
-      <c r="D263" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E263" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F263" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="264" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A264" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="B264" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="C264" s="34">
-        <v>1999</v>
-      </c>
-      <c r="D264" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E264" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F264" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="265" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A265" s="31" t="s">
-        <v>37</v>
-      </c>
-      <c r="B265" s="31" t="s">
-        <v>131</v>
-      </c>
-      <c r="C265" s="34">
-        <v>2000</v>
-      </c>
-      <c r="D265" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E265" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F265" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="266" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A266" s="31" t="s">
-        <v>133</v>
-      </c>
-      <c r="B266" s="31" t="s">
-        <v>132</v>
-      </c>
-      <c r="C266" s="34">
-        <v>2001</v>
-      </c>
-      <c r="D266" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E266" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F266" s="32" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="267" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A267" s="31" t="s">
-        <v>15</v>
-      </c>
-      <c r="B267" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C267" s="34">
-        <v>1999</v>
-      </c>
-      <c r="D267" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E267" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F267" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="268" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A268" s="31" t="s">
-        <v>17</v>
-      </c>
-      <c r="B268" s="31" t="s">
-        <v>16</v>
-      </c>
-      <c r="C268" s="34">
-        <v>1998</v>
-      </c>
-      <c r="D268" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E268" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F268" s="32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="269" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A269" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="B269" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="C269" s="40">
-        <v>2000</v>
-      </c>
-      <c r="D269" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E269" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F269" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="270" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A270" s="38" t="s">
-        <v>167</v>
-      </c>
-      <c r="B270" s="38" t="s">
-        <v>166</v>
-      </c>
-      <c r="C270" s="40">
-        <v>1999</v>
-      </c>
-      <c r="D270" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E270" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F270" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="271" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A271" s="38" t="s">
-        <v>9</v>
-      </c>
-      <c r="B271" s="38" t="s">
-        <v>168</v>
-      </c>
-      <c r="C271" s="41">
-        <v>1998</v>
-      </c>
-      <c r="D271" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E271" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F271" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="272" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A272" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="B272" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="C272" s="41">
-        <v>1998</v>
-      </c>
-      <c r="D272" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E272" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F272" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="273" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A273" s="48" t="s">
-        <v>170</v>
-      </c>
-      <c r="B273" s="48" t="s">
-        <v>169</v>
-      </c>
-      <c r="C273" s="41">
-        <v>1999</v>
-      </c>
-      <c r="D273" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E273" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F273" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="274" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A274" s="49" t="s">
-        <v>110</v>
-      </c>
-      <c r="B274" s="49" t="s">
-        <v>169</v>
-      </c>
-      <c r="C274" s="50">
-        <v>1997</v>
-      </c>
-      <c r="D274" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E274" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F274" s="39" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="275" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A275" s="18" t="s">
-        <v>37</v>
-      </c>
-      <c r="B275" s="18" t="s">
-        <v>36</v>
-      </c>
-      <c r="C275" s="47">
-        <v>1996</v>
-      </c>
-      <c r="D275" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E275" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F275" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="276" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A276" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="B276" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="C276" s="30">
-        <v>1997</v>
-      </c>
-      <c r="D276" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E276" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F276" s="19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="277" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A277" s="22" t="s">
-        <v>208</v>
-      </c>
-      <c r="B277" s="22" t="s">
-        <v>207</v>
-      </c>
-      <c r="C277" s="24">
-        <v>1998</v>
-      </c>
-      <c r="D277" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E277" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F277" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="278" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A278" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="B278" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="C278" s="24">
-        <v>2000</v>
-      </c>
-      <c r="D278" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E278" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F278" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="279" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A279" s="22" t="s">
-        <v>56</v>
-      </c>
-      <c r="B279" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C279" s="24">
-        <v>1998</v>
-      </c>
-      <c r="D279" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E279" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F279" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="280" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A280" s="22" t="s">
-        <v>203</v>
-      </c>
-      <c r="B280" s="22" t="s">
-        <v>211</v>
-      </c>
-      <c r="C280" s="24">
-        <v>1998</v>
-      </c>
-      <c r="D280" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E280" s="23" t="s">
-        <v>216</v>
-      </c>
-      <c r="F280" s="19" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="281" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A281" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="B281" s="10" t="s">
-        <v>62</v>
-      </c>
-      <c r="C281" s="12">
-        <v>1999</v>
-      </c>
-      <c r="D281" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E281" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F281" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="282" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A282" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B282" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="C282" s="14">
-        <v>1998</v>
-      </c>
-      <c r="D282" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E282" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F282" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="283" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B283" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C283" s="14">
-        <v>1996</v>
-      </c>
-      <c r="D283" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E283" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F283" s="11" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="284" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A284" s="28" t="s">
-        <v>68</v>
-      </c>
-      <c r="B284" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="C284" s="29">
-        <v>1997</v>
-      </c>
-      <c r="D284" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E284" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F284" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="285" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A285" s="28" t="s">
-        <v>70</v>
-      </c>
-      <c r="B285" s="28" t="s">
-        <v>69</v>
-      </c>
-      <c r="C285" s="29">
-        <v>1997</v>
-      </c>
-      <c r="D285" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E285" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F285" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="286" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A286" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B286" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="C286" s="29">
-        <v>1995</v>
-      </c>
-      <c r="D286" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E286" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F286" s="26" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="287" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A287" s="52" t="s">
-        <v>87</v>
-      </c>
-      <c r="B287" s="52" t="s">
-        <v>86</v>
-      </c>
-      <c r="C287" s="46">
-        <v>1996</v>
-      </c>
-      <c r="D287" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E287" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F287" s="33" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="288" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A288" s="53" t="s">
-        <v>88</v>
-      </c>
-      <c r="B288" s="53" t="s">
-        <v>75</v>
-      </c>
-      <c r="C288" s="37">
-        <v>1996</v>
-      </c>
-      <c r="D288" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E288" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F288" s="32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="289" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A289" s="49" t="s">
-        <v>137</v>
-      </c>
-      <c r="B289" s="49" t="s">
-        <v>213</v>
-      </c>
-      <c r="C289" s="41">
-        <v>1998</v>
-      </c>
-      <c r="D289" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E289" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F289" s="39" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="290" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A290" s="59" t="s">
-        <v>135</v>
-      </c>
-      <c r="B290" s="59" t="s">
-        <v>134</v>
-      </c>
-      <c r="C290" s="61">
-        <v>1996</v>
-      </c>
-      <c r="D290" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E290" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F290" s="60" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="291" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A291" s="59" t="s">
-        <v>56</v>
-      </c>
-      <c r="B291" s="59" t="s">
-        <v>136</v>
-      </c>
-      <c r="C291" s="61">
-        <v>1996</v>
-      </c>
-      <c r="D291" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E291" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F291" s="62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="292" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A292" s="59" t="s">
-        <v>73</v>
-      </c>
-      <c r="B292" s="59" t="s">
-        <v>46</v>
-      </c>
-      <c r="C292" s="61">
-        <v>1997</v>
-      </c>
-      <c r="D292" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E292" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F292" s="62" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="293" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A293" s="54" t="s">
-        <v>139</v>
-      </c>
-      <c r="B293" s="54" t="s">
-        <v>138</v>
-      </c>
-      <c r="C293" s="57">
-        <v>1998</v>
-      </c>
-      <c r="D293" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E293" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F293" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="294" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A294" s="54" t="s">
-        <v>140</v>
-      </c>
-      <c r="B294" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C294" s="57">
-        <v>1998</v>
-      </c>
-      <c r="D294" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E294" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F294" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="295" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A295" s="54" t="s">
-        <v>141</v>
-      </c>
-      <c r="B295" s="54" t="s">
-        <v>89</v>
-      </c>
-      <c r="C295" s="57">
-        <v>1999</v>
-      </c>
-      <c r="D295" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E295" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F295" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="296" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A296" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="B296" s="54" t="s">
-        <v>27</v>
-      </c>
-      <c r="C296" s="58">
-        <v>1999</v>
-      </c>
-      <c r="D296" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="E296" s="56" t="s">
-        <v>215</v>
-      </c>
-      <c r="F296" s="55" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="297" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A297" s="63" t="s">
-        <v>220</v>
-      </c>
-      <c r="B297" s="63" t="s">
-        <v>221</v>
-      </c>
-      <c r="C297" s="64">
-        <v>1994</v>
-      </c>
-      <c r="D297" s="65" t="s">
-        <v>214</v>
-      </c>
-      <c r="E297" s="66" t="s">
-        <v>215</v>
-      </c>
-      <c r="F297" s="67" t="s">
         <v>90</v>
       </c>
     </row>

</xml_diff>